<commit_message>
Atualização da capa e do background. Adicionado o valor institucional 1,00 ao SEAP.
</commit_message>
<xml_diff>
--- a/Inventário de Ativos Intangíveis/2024/3. Analise de Dados/3.2. Dados/Dados.xlsx
+++ b/Inventário de Ativos Intangíveis/2024/3. Analise de Dados/3.2. Dados/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Seplag\Inventário de Ativos Intangíveis\2024\3. Analise de Dados\3.2. Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3064D4-64C1-47C9-81A1-2AAE9500D072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89576EC6-EFD7-4538-906E-DBCF48DE49AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -809,7 +809,7 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3102,7 +3102,9 @@
       <c r="H50" s="17"/>
       <c r="I50" s="13"/>
       <c r="J50" s="18"/>
-      <c r="K50" s="15"/>
+      <c r="K50" s="15">
+        <v>1</v>
+      </c>
       <c r="L50" s="18">
         <v>96833.33</v>
       </c>

</xml_diff>